<commit_message>
summary: committing the windows mobile 7 library components
</commit_message>
<xml_diff>
--- a/PushNotification/Documents/Push Notification Component.xlsx
+++ b/PushNotification/Documents/Push Notification Component.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="14355" windowHeight="4680" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="14355" windowHeight="4680" tabRatio="696"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,93 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
+    <t>Deliverables</t>
+  </si>
+  <si>
+    <t>S#</t>
+  </si>
+  <si>
+    <t>Exclusions</t>
+  </si>
+  <si>
+    <t>Artifact Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Out of Scope </t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Project to be created on Github</t>
+  </si>
+  <si>
+    <t>Interfaces</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Use Cases</t>
+  </si>
+  <si>
+    <t>Source code in github</t>
+  </si>
+  <si>
+    <t>Push Notification Module</t>
+  </si>
+  <si>
+    <t>Application registers on the server</t>
+  </si>
+  <si>
+    <t>Application unregisters on the server</t>
+  </si>
+  <si>
+    <t>Serial No.</t>
+  </si>
+  <si>
+    <t>Application Registers to the server</t>
+  </si>
+  <si>
+    <t>Application Un Registers from the server</t>
+  </si>
+  <si>
+    <t>Device gets notification after Un Registration</t>
+  </si>
+  <si>
+    <t>Notification is displayed</t>
+  </si>
+  <si>
+    <t>Unit Testing is excluded because of the use of 3rd party server</t>
+  </si>
+  <si>
+    <t>Device gets notification on successful Registration</t>
+  </si>
+  <si>
+    <t>Notification is displayed on receiving message from server when application is not running</t>
+  </si>
+  <si>
+    <t>Notification is displayed on receiving message from server when application is running</t>
+  </si>
+  <si>
+    <t>Notification is handled and a message box is displayed with  notification contents</t>
+  </si>
+  <si>
+    <t>Application tries to Register/Un Register from the server when internet is not available.</t>
+  </si>
+  <si>
+    <t>Notification is displayed on receiving message from server when application is running.</t>
+  </si>
+  <si>
+    <t>Notification is displayed on receiving message from server when application is not running.</t>
+  </si>
+  <si>
+    <t>Message Box with connection error message is shown.</t>
+  </si>
+  <si>
+    <t>Notification is handled and a message box is displayed with push notification contents</t>
+  </si>
+  <si>
     <r>
       <t>Contact:</t>
     </r>
@@ -31,95 +118,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> pankaj.c@optimusinfo.com</t>
+      <t xml:space="preserve"> Anubhav Gupta (anubhav.gupta@optimusinfo.com)</t>
     </r>
-  </si>
-  <si>
-    <t>Deliverables</t>
-  </si>
-  <si>
-    <t>S#</t>
-  </si>
-  <si>
-    <t>Exclusions</t>
-  </si>
-  <si>
-    <t>Artifact Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Out of Scope </t>
-  </si>
-  <si>
-    <t>Module</t>
-  </si>
-  <si>
-    <t>Project to be created on Github</t>
-  </si>
-  <si>
-    <t>Interfaces</t>
-  </si>
-  <si>
-    <t>Remarks</t>
-  </si>
-  <si>
-    <t>Use Cases</t>
-  </si>
-  <si>
-    <t>Source code in github</t>
-  </si>
-  <si>
-    <t>Push Notification Module</t>
-  </si>
-  <si>
-    <t>Application registers on the server</t>
-  </si>
-  <si>
-    <t>Application unregisters on the server</t>
-  </si>
-  <si>
-    <t>Serial No.</t>
-  </si>
-  <si>
-    <t>Application Registers to the server</t>
-  </si>
-  <si>
-    <t>Application Un Registers from the server</t>
-  </si>
-  <si>
-    <t>Device gets notification after Un Registration</t>
-  </si>
-  <si>
-    <t>Notification is displayed</t>
-  </si>
-  <si>
-    <t>Unit Testing is excluded because of the use of 3rd party server</t>
-  </si>
-  <si>
-    <t>Device gets notification on successful Registration</t>
-  </si>
-  <si>
-    <t>Notification is displayed on receiving message from server when application is not running</t>
-  </si>
-  <si>
-    <t>Notification is displayed on receiving message from server when application is running</t>
-  </si>
-  <si>
-    <t>Notification is handled and a message box is displayed with  notification contents</t>
-  </si>
-  <si>
-    <t>Application tries to Register/Un Register from the server when internet is not available.</t>
-  </si>
-  <si>
-    <t>Notification is displayed on receiving message from server when application is running.</t>
-  </si>
-  <si>
-    <t>Notification is displayed on receiving message from server when application is not running.</t>
-  </si>
-  <si>
-    <t>Message Box with connection error message is shown.</t>
-  </si>
-  <si>
-    <t>Notification is handled and a message box is displayed with push notification contents</t>
   </si>
 </sst>
 </file>
@@ -349,23 +349,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -455,31 +443,31 @@
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:axId val="53901568"/>
-        <c:axId val="53923200"/>
+        <c:axId val="32715520"/>
+        <c:axId val="32717056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="53901568"/>
+        <c:axId val="32715520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53923200"/>
+        <c:crossAx val="32717056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53923200"/>
+        <c:axId val="32717056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53901568"/>
+        <c:crossAx val="32715520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -504,31 +492,31 @@
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:axId val="59374976"/>
-        <c:axId val="70313088"/>
+        <c:axId val="32798976"/>
+        <c:axId val="32813056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="59374976"/>
+        <c:axId val="32798976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70313088"/>
+        <c:crossAx val="32813056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70313088"/>
+        <c:axId val="32813056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59374976"/>
+        <c:crossAx val="32798976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -550,7 +538,8 @@
     <sheetView zoomScale="116" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </chartsheet>
 </file>
 
@@ -1063,44 +1052,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="4" spans="1:7">
-      <c r="A4" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
+      <c r="A4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
     </row>
     <row r="5" spans="1:7" ht="24.75" customHeight="1">
-      <c r="A5" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
+      <c r="A5" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
+      <c r="A8" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1117,59 +1106,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="83.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="79.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="83.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="79.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="9">
         <v>2</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="13">
-        <v>1</v>
-      </c>
-      <c r="B2" s="13" t="s">
+      <c r="B3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="13">
-        <v>2</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="14">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1177,10 +1166,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1204,14 +1193,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="16" t="s">
+      <c r="A1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>9</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1219,10 +1208,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1230,10 +1219,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
         <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1241,10 +1230,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1252,10 +1241,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1263,10 +1252,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1279,149 +1268,152 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="47.5703125" customWidth="1"/>
-    <col min="5" max="5" width="66.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="47.42578125" style="2" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="2"/>
+    <col min="5" max="5" width="46.5703125" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="17"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="20" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="21"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.75">
-      <c r="A2" s="6" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="4"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="4">
+        <v>3</v>
+      </c>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="4"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="4">
         <v>4</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="8">
-        <v>1</v>
-      </c>
-      <c r="B3" s="11" t="s">
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="4"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="4">
+        <v>6</v>
+      </c>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="4"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="4">
         <v>7</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="8">
-        <v>1</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="8">
-        <v>2</v>
-      </c>
-      <c r="B4" s="11" t="s">
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="4"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="4">
+        <v>8</v>
+      </c>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="4"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="4">
+        <v>9</v>
+      </c>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="4"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="4">
+        <v>10</v>
+      </c>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="4"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="4">
         <v>11</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="8">
-        <v>2</v>
-      </c>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="8"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="8">
-        <v>3</v>
-      </c>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="8"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="8">
-        <v>4</v>
-      </c>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="8"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="8">
-        <v>5</v>
-      </c>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="8"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="8">
-        <v>6</v>
-      </c>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="8"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="8">
-        <v>7</v>
-      </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="8"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="8">
-        <v>8</v>
-      </c>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="8"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="8">
-        <v>9</v>
-      </c>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="8"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="8">
-        <v>10</v>
-      </c>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="8"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="8">
-        <v>11</v>
-      </c>
-      <c r="E13" s="5"/>
+      <c r="E13" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1429,5 +1421,6 @@
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>